<commit_message>
Added some changes to investments after more stocks bought and iPin raise
</commit_message>
<xml_diff>
--- a/finansiele berekeninge 2015.xlsx
+++ b/finansiele berekeninge 2015.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shizuka\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\Umbopo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92C1660C-C716-4942-90B4-F4FEAB8BE941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C173EF-BE9E-45BE-BF27-C43F1A1D10A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-4680" windowWidth="29040" windowHeight="15840" tabRatio="695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SALARIS" sheetId="22" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2026" uniqueCount="663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2036" uniqueCount="673">
   <si>
     <t>Maandlikse salaris</t>
   </si>
@@ -2030,10 +2030,40 @@
     <t>Moet 6k hou vir kar regmaak (koppelaar)</t>
   </si>
   <si>
-    <t>9k</t>
-  </si>
-  <si>
     <t>Bêre vir die volgende lendevrug</t>
+  </si>
+  <si>
+    <t>19k</t>
+  </si>
+  <si>
+    <t>Nuwe Creepy en Swembad 3k</t>
+  </si>
+  <si>
+    <t>Ore en brill vir skiet, met ore kassies 2k</t>
+  </si>
+  <si>
+    <t>SHARE Purchase</t>
+  </si>
+  <si>
+    <t> BUY 25 ETF5IT @ 21.00 - ORDER# 5</t>
+  </si>
+  <si>
+    <t>GLN CAPITAL D - DIVIDEND PAYOUT</t>
+  </si>
+  <si>
+    <t>Money transfer (Was 10, maar 5 terug omdat nie Krugerrand kan koop met SHARES ZERO NIE</t>
+  </si>
+  <si>
+    <t>BUY 10 GLN @ 106.17 - ORDER# 7</t>
+  </si>
+  <si>
+    <t>BUY 40 OMU @ 12.29 - ORDER# 8</t>
+  </si>
+  <si>
+    <t>BEGIN OP 3 Mei 2023</t>
+  </si>
+  <si>
+    <t>MOES TEGNIES AL BEGIN HET TOE SY GEBORE WAS</t>
   </si>
 </sst>
 </file>
@@ -3396,7 +3426,7 @@
     <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="359">
+  <cellXfs count="360">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="15" xfId="3" applyBorder="1"/>
@@ -4114,6 +4144,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="20">
     <cellStyle name="20% - Accent2" xfId="19" builtinId="34"/>
@@ -4350,7 +4383,7 @@
                   <c:v>48929.4</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>48929.4</c:v>
+                  <c:v>52354.458000000006</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>54500</c:v>
@@ -5518,10 +5551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D37CFB-3750-4140-B070-A288E4BD3B86}">
-  <dimension ref="B2:Z53"/>
+  <dimension ref="B2:AA59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="Y26" sqref="Y26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5529,7 +5562,7 @@
     <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.42578125" customWidth="1"/>
     <col min="14" max="14" width="7" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="17.28515625" bestFit="1" customWidth="1"/>
@@ -5570,7 +5603,7 @@
         <v>649</v>
       </c>
       <c r="Q4" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="R4" t="s">
         <v>650</v>
@@ -5596,7 +5629,7 @@
         <v>59</v>
       </c>
       <c r="T5" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
     </row>
     <row r="6" spans="2:26">
@@ -5689,6 +5722,9 @@
       <c r="C13">
         <v>36617.354169999999</v>
       </c>
+      <c r="R13" t="s">
+        <v>663</v>
+      </c>
     </row>
     <row r="14" spans="2:26">
       <c r="B14">
@@ -5697,6 +5733,9 @@
       <c r="C14">
         <v>42465.77</v>
       </c>
+      <c r="R14" t="s">
+        <v>664</v>
+      </c>
       <c r="W14" t="s">
         <v>32</v>
       </c>
@@ -5738,7 +5777,7 @@
         <v>45893.11</v>
       </c>
     </row>
-    <row r="17" spans="2:26">
+    <row r="17" spans="2:27">
       <c r="B17">
         <v>2022</v>
       </c>
@@ -5746,15 +5785,20 @@
         <v>48929.4</v>
       </c>
     </row>
-    <row r="18" spans="2:26">
+    <row r="18" spans="2:27">
       <c r="B18">
         <v>2023</v>
       </c>
       <c r="C18">
-        <v>48929.4</v>
-      </c>
-    </row>
-    <row r="19" spans="2:26">
+        <f>48929.4*1.07</f>
+        <v>52354.458000000006</v>
+      </c>
+      <c r="D18">
+        <f>C18-C17</f>
+        <v>3425.0580000000045</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27">
       <c r="B19">
         <v>2024</v>
       </c>
@@ -5762,7 +5806,7 @@
         <v>54500</v>
       </c>
     </row>
-    <row r="20" spans="2:26">
+    <row r="20" spans="2:27">
       <c r="B20">
         <v>2025</v>
       </c>
@@ -5770,7 +5814,7 @@
         <v>58500</v>
       </c>
     </row>
-    <row r="21" spans="2:26">
+    <row r="21" spans="2:27">
       <c r="B21">
         <v>2026</v>
       </c>
@@ -5778,7 +5822,7 @@
         <v>63000</v>
       </c>
     </row>
-    <row r="22" spans="2:26">
+    <row r="22" spans="2:27">
       <c r="B22">
         <v>2027</v>
       </c>
@@ -5788,11 +5832,16 @@
       <c r="W22" s="26" t="s">
         <v>621</v>
       </c>
-      <c r="X22" s="26"/>
-      <c r="Y22" s="26"/>
-      <c r="Z22" s="26"/>
-    </row>
-    <row r="23" spans="2:26">
+      <c r="X22" s="351" t="s">
+        <v>671</v>
+      </c>
+      <c r="Y22" s="351"/>
+      <c r="Z22" s="351"/>
+      <c r="AA22" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="23" spans="2:27">
       <c r="B23">
         <v>2028</v>
       </c>
@@ -5812,7 +5861,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="24" spans="2:26" ht="23.25">
+    <row r="24" spans="2:27" ht="23.25">
       <c r="B24" s="251" t="s">
         <v>602</v>
       </c>
@@ -5835,14 +5884,14 @@
         <v>100</v>
       </c>
       <c r="Y24">
-        <v>200</v>
+        <v>5000</v>
       </c>
       <c r="Z24">
         <f>Y24+(X24*12)</f>
-        <v>1400</v>
-      </c>
-    </row>
-    <row r="25" spans="2:26">
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27">
       <c r="C25" s="180" t="s">
         <v>600</v>
       </c>
@@ -5852,9 +5901,9 @@
       <c r="E25" s="180" t="s">
         <v>603</v>
       </c>
-      <c r="M25" s="180">
-        <f>48929.4</f>
-        <v>48929.4</v>
+      <c r="M25">
+        <f>48929.4*1.07</f>
+        <v>52354.458000000006</v>
       </c>
       <c r="N25" s="180" t="s">
         <v>236</v>
@@ -5866,17 +5915,17 @@
         <v>2</v>
       </c>
       <c r="X25">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="Y25">
         <v>1000</v>
       </c>
       <c r="Z25">
         <f t="shared" ref="Z25:Z30" si="0">Z24+Y25++(X25*12)</f>
-        <v>5400</v>
-      </c>
-    </row>
-    <row r="26" spans="2:26">
+        <v>11400</v>
+      </c>
+    </row>
+    <row r="26" spans="2:27">
       <c r="D26" t="s">
         <v>596</v>
       </c>
@@ -5888,7 +5937,7 @@
       </c>
       <c r="M26">
         <f>M25*0.3</f>
-        <v>14678.82</v>
+        <v>15706.3374</v>
       </c>
       <c r="N26" t="s">
         <v>607</v>
@@ -5898,23 +5947,23 @@
       </c>
       <c r="T26">
         <f>S26/M25*100</f>
-        <v>40.33625999910074</v>
+        <v>37.697439251496021</v>
       </c>
       <c r="W26">
         <v>3</v>
       </c>
       <c r="X26">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="Y26">
         <v>1000</v>
       </c>
       <c r="Z26">
         <f t="shared" si="0"/>
-        <v>9400</v>
-      </c>
-    </row>
-    <row r="27" spans="2:26">
+        <v>16600</v>
+      </c>
+    </row>
+    <row r="27" spans="2:27">
       <c r="B27" s="242">
         <v>44835</v>
       </c>
@@ -5934,7 +5983,7 @@
       </c>
       <c r="M27">
         <f>M25*0.15</f>
-        <v>7339.41</v>
+        <v>7853.1687000000002</v>
       </c>
       <c r="N27" t="s">
         <v>608</v>
@@ -5944,23 +5993,23 @@
       </c>
       <c r="T27">
         <f>S27/M25*100</f>
-        <v>12.262566064574672</v>
+        <v>11.460342116424926</v>
       </c>
       <c r="W27">
         <v>4</v>
       </c>
       <c r="X27">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="Y27">
         <v>1000</v>
       </c>
       <c r="Z27">
         <f t="shared" si="0"/>
-        <v>13400</v>
-      </c>
-    </row>
-    <row r="28" spans="2:26">
+        <v>21800</v>
+      </c>
+    </row>
+    <row r="28" spans="2:27">
       <c r="B28" s="242">
         <v>44866</v>
       </c>
@@ -5980,7 +6029,7 @@
       </c>
       <c r="M28">
         <f>M25*0.15</f>
-        <v>7339.41</v>
+        <v>7853.1687000000002</v>
       </c>
       <c r="N28" t="s">
         <v>609</v>
@@ -5991,23 +6040,23 @@
       </c>
       <c r="T28">
         <f>S28/M25*100</f>
-        <v>7.0414311232101765</v>
+        <v>6.5807767506637154</v>
       </c>
       <c r="W28">
         <v>5</v>
       </c>
       <c r="X28">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="Y28">
         <v>1000</v>
       </c>
       <c r="Z28">
         <f t="shared" si="0"/>
-        <v>17400</v>
-      </c>
-    </row>
-    <row r="29" spans="2:26">
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="29" spans="2:27">
       <c r="B29" s="242">
         <v>44896</v>
       </c>
@@ -6030,7 +6079,7 @@
       </c>
       <c r="M29">
         <f>M25*0.2</f>
-        <v>9785.880000000001</v>
+        <v>10470.891600000003</v>
       </c>
       <c r="N29" t="s">
         <v>610</v>
@@ -6041,23 +6090,23 @@
       </c>
       <c r="T29">
         <f>S29/M25*100</f>
-        <v>6.6903742943915105</v>
+        <v>6.2526862564406631</v>
       </c>
       <c r="W29">
         <v>6</v>
       </c>
       <c r="X29">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="Y29">
         <v>1000</v>
       </c>
       <c r="Z29">
         <f t="shared" si="0"/>
-        <v>21400</v>
-      </c>
-    </row>
-    <row r="30" spans="2:26">
+        <v>32200</v>
+      </c>
+    </row>
+    <row r="30" spans="2:27">
       <c r="B30" s="242">
         <v>44927</v>
       </c>
@@ -6077,7 +6126,7 @@
       </c>
       <c r="M30">
         <f>M25*0.1</f>
-        <v>4892.9400000000005</v>
+        <v>5235.4458000000013</v>
       </c>
       <c r="N30" t="s">
         <v>611</v>
@@ -6087,23 +6136,23 @@
       </c>
       <c r="T30">
         <f>S30/M25*100</f>
-        <v>5.3137786279823578</v>
+        <v>4.9661482504508019</v>
       </c>
       <c r="W30">
         <v>7</v>
       </c>
       <c r="X30">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="Y30">
         <v>1000</v>
       </c>
       <c r="Z30">
         <f t="shared" si="0"/>
-        <v>25400</v>
-      </c>
-    </row>
-    <row r="31" spans="2:26">
+        <v>37400</v>
+      </c>
+    </row>
+    <row r="31" spans="2:27">
       <c r="B31" s="242">
         <v>44958</v>
       </c>
@@ -6123,7 +6172,7 @@
       </c>
       <c r="M31">
         <f>M25*0.05</f>
-        <v>2446.4700000000003</v>
+        <v>2617.7229000000007</v>
       </c>
       <c r="N31" t="s">
         <v>612</v>
@@ -6134,23 +6183,23 @@
       </c>
       <c r="T31">
         <f>S31/M25*100</f>
-        <v>10.451385056836994</v>
+        <v>9.7676495858289645</v>
       </c>
       <c r="W31">
         <v>8</v>
       </c>
       <c r="X31">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="Y31">
         <v>1000</v>
       </c>
       <c r="Z31">
         <f t="shared" ref="Z31:Z32" si="3">Z30+Y31++(X31*12)</f>
-        <v>29400</v>
-      </c>
-    </row>
-    <row r="32" spans="2:26">
+        <v>42600</v>
+      </c>
+    </row>
+    <row r="32" spans="2:27">
       <c r="B32" s="242">
         <v>44986</v>
       </c>
@@ -6173,7 +6222,7 @@
       </c>
       <c r="M32">
         <f>M25*0.05</f>
-        <v>2446.4700000000003</v>
+        <v>2617.7229000000007</v>
       </c>
       <c r="N32" t="s">
         <v>614</v>
@@ -6184,20 +6233,20 @@
       </c>
       <c r="T32">
         <f>S32/M25*100</f>
-        <v>2.7590773645293014</v>
+        <v>2.5785769761956083</v>
       </c>
       <c r="W32">
         <v>9</v>
       </c>
       <c r="X32">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="Y32">
         <v>1000</v>
       </c>
       <c r="Z32">
         <f t="shared" si="3"/>
-        <v>33400</v>
+        <v>47800</v>
       </c>
     </row>
     <row r="33" spans="2:26">
@@ -6209,20 +6258,26 @@
       </c>
       <c r="T33">
         <f>M25-SUM(S26:S32)</f>
-        <v>7410.419999999991</v>
+        <v>10835.477999999996</v>
       </c>
       <c r="W33">
         <v>10</v>
       </c>
       <c r="X33">
-        <v>250</v>
+        <v>350</v>
       </c>
       <c r="Y33">
         <v>1000</v>
       </c>
       <c r="Z33">
         <f t="shared" ref="Z33" si="4">Z32+Y33++(X33*12)</f>
-        <v>37400</v>
+        <v>53000</v>
+      </c>
+    </row>
+    <row r="35" spans="2:26">
+      <c r="F35">
+        <f>48929.4*1.07</f>
+        <v>52354.458000000006</v>
       </c>
     </row>
     <row r="37" spans="2:26">
@@ -6260,7 +6315,7 @@
     <row r="43" spans="2:26">
       <c r="D43">
         <f>SUM(C46:C1048576)</f>
-        <v>3000</v>
+        <v>8581.09</v>
       </c>
       <c r="G43">
         <f>2976.76+121.59</f>
@@ -6271,6 +6326,10 @@
       <c r="B44" t="s">
         <v>638</v>
       </c>
+      <c r="D44">
+        <f>SUM(C46:C1000)</f>
+        <v>8581.09</v>
+      </c>
     </row>
     <row r="45" spans="2:26">
       <c r="C45" t="s">
@@ -6360,10 +6419,80 @@
         <v>500</v>
       </c>
     </row>
+    <row r="54" spans="2:5">
+      <c r="B54" s="250">
+        <v>45113</v>
+      </c>
+      <c r="D54" s="44" t="s">
+        <v>665</v>
+      </c>
+      <c r="E54">
+        <v>9.66</v>
+      </c>
+    </row>
+    <row r="55" spans="2:5">
+      <c r="B55" s="250">
+        <v>45113</v>
+      </c>
+      <c r="C55">
+        <v>525</v>
+      </c>
+      <c r="D55" s="44" t="s">
+        <v>666</v>
+      </c>
+      <c r="E55">
+        <v>534.66</v>
+      </c>
+    </row>
+    <row r="56" spans="2:5">
+      <c r="B56" s="250">
+        <v>45191</v>
+      </c>
+      <c r="C56">
+        <v>56.09</v>
+      </c>
+      <c r="D56" s="44" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="57" spans="2:5" ht="39">
+      <c r="B57" s="250">
+        <v>45215</v>
+      </c>
+      <c r="C57">
+        <v>5000</v>
+      </c>
+      <c r="D57" s="359" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="58" spans="2:5">
+      <c r="B58" s="250">
+        <v>45215</v>
+      </c>
+      <c r="D58" s="44" t="s">
+        <v>669</v>
+      </c>
+      <c r="E58">
+        <v>1075.56</v>
+      </c>
+    </row>
+    <row r="59" spans="2:5">
+      <c r="B59" s="250">
+        <v>45215</v>
+      </c>
+      <c r="D59" s="44" t="s">
+        <v>670</v>
+      </c>
+      <c r="E59">
+        <v>502.39</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="B24:F24"/>
     <mergeCell ref="M24:O24"/>
+    <mergeCell ref="X22:Z22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -19508,7 +19637,7 @@
   <dimension ref="A1:AF111"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19598,7 +19727,7 @@
     </row>
     <row r="2" spans="1:31" ht="16.5" thickTop="1" thickBot="1">
       <c r="A2" s="281">
-        <v>48929.4</v>
+        <v>52354.46</v>
       </c>
       <c r="B2" s="282"/>
       <c r="C2" s="191"/>
@@ -19670,7 +19799,9 @@
     </row>
     <row r="3" spans="1:31" ht="16.5" thickTop="1" thickBot="1">
       <c r="A3" s="26"/>
-      <c r="B3" s="47"/>
+      <c r="B3" s="47">
+        <v>52354.46</v>
+      </c>
       <c r="C3" s="191"/>
       <c r="D3" s="191">
         <v>2891.88</v>
@@ -19729,7 +19860,7 @@
       </c>
       <c r="I4" s="47">
         <f>A2*0.3</f>
-        <v>14678.82</v>
+        <v>15706.338</v>
       </c>
       <c r="K4" s="270" t="s">
         <v>504</v>
@@ -20770,15 +20901,15 @@
       </c>
       <c r="C37" s="154">
         <f>A2-C36</f>
-        <v>5099.7000000000044</v>
+        <v>8524.760000000002</v>
       </c>
       <c r="D37" s="154">
         <f>A2-D36</f>
-        <v>1195.0499999999956</v>
+        <v>4620.1099999999933</v>
       </c>
       <c r="E37" s="144">
         <f>A2-E36+E29</f>
-        <v>3700.3600000000006</v>
+        <v>7125.4199999999983</v>
       </c>
       <c r="H37" s="47"/>
       <c r="I37" s="47"/>

</xml_diff>

<commit_message>
Papiere en finansies opdatering
</commit_message>
<xml_diff>
--- a/finansiele berekeninge 2015.xlsx
+++ b/finansiele berekeninge 2015.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repo\Umbopo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBED1D57-C842-4A1B-BBC7-688593BBE5AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F79BC9C2-CA5E-4031-883B-11873B5BBD78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="695" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SALARIS" sheetId="22" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2054" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="700">
   <si>
     <t>Maandlikse salaris</t>
   </si>
@@ -2054,9 +2054,6 @@
     <t>MOES TEGNIES AL BEGIN HET TOE SY GEBORE WAS</t>
   </si>
   <si>
-    <t>Money transfer (Was 10k, maar 5k terug omdat nie Krugerrand kan koop met SHARES ZERO</t>
-  </si>
-  <si>
     <t>Omu Cash Div @ZAR0,32 p/s</t>
   </si>
   <si>
@@ -2066,9 +2063,6 @@
     <t>ELYSSA - KOS en R2000 se speelgeld</t>
   </si>
   <si>
-    <t>SAV1: 1250 SAV2: 750 INV: 500 texfree: 300</t>
-  </si>
-  <si>
     <t>Whyness</t>
   </si>
   <si>
@@ -2121,6 +2115,36 @@
   </si>
   <si>
     <t>POSITIVE MEANS GAIN</t>
+  </si>
+  <si>
+    <t>BUY 20 IMP @ 70,39 - ORDER# 9</t>
+  </si>
+  <si>
+    <t>Impala Platinum</t>
+  </si>
+  <si>
+    <t>Aftreeaftrekking</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAV1: 1250 SAV2: 750 INV: 500 </t>
+  </si>
+  <si>
+    <t>taxfree: 300</t>
+  </si>
+  <si>
+    <t>10x S&amp;p 500</t>
+  </si>
+  <si>
+    <t>Climbed</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>BUY 20 CSP500 (10x S&amp;p500)@ 87.36.</t>
+  </si>
+  <si>
+    <t>Money transfer (Was 10k, maar 5k terug omdat nie Krugerrand kan koop met SHARES ZERO)</t>
   </si>
 </sst>
 </file>
@@ -5192,16 +5216,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5609,10 +5633,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12D37CFB-3750-4140-B070-A288E4BD3B86}">
-  <dimension ref="B2:AA62"/>
+  <dimension ref="B1:AC65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="M44" sqref="M44"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="L50" sqref="L50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5621,892 +5645,1045 @@
     <col min="2" max="2" width="10.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" customWidth="1"/>
-    <col min="15" max="15" width="7" customWidth="1"/>
-    <col min="16" max="16" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" customWidth="1"/>
+    <col min="16" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" customWidth="1"/>
+    <col min="20" max="21" width="10" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:26">
+    <row r="1" spans="2:28">
+      <c r="D1">
+        <f>AVERAGE(D4:D18)</f>
+        <v>3146.748</v>
+      </c>
+    </row>
+    <row r="2" spans="2:28">
       <c r="B2" s="180" t="s">
         <v>593</v>
       </c>
       <c r="C2" s="180" t="s">
         <v>594</v>
       </c>
-    </row>
-    <row r="3" spans="2:26">
+      <c r="D2" t="s">
+        <v>696</v>
+      </c>
+      <c r="E2" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="3" spans="2:28">
       <c r="B3" s="180">
         <v>2008</v>
       </c>
       <c r="C3" s="180">
         <v>5000</v>
       </c>
-      <c r="P3" t="s">
+      <c r="D3" s="180"/>
+      <c r="R3" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="4" spans="2:26">
+    <row r="4" spans="2:28">
       <c r="B4">
         <v>2009</v>
       </c>
       <c r="C4" s="42">
         <v>11800</v>
       </c>
-      <c r="P4" t="s">
+      <c r="D4" s="42">
+        <f t="shared" ref="D4:D18" si="0">C4-C3</f>
+        <v>6800</v>
+      </c>
+      <c r="E4">
+        <f>D4/C3*100</f>
+        <v>136</v>
+      </c>
+      <c r="R4" t="s">
         <v>648</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>660</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>649</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
         <v>652</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="5" spans="2:26">
+    <row r="5" spans="2:28">
       <c r="B5">
         <v>2010</v>
       </c>
       <c r="C5" s="42">
         <v>12500</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="D5" s="42">
+        <f t="shared" si="0"/>
+        <v>700</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ref="E5:E18" si="1">D5/C4*100</f>
+        <v>5.9322033898305087</v>
+      </c>
+      <c r="S5" t="s">
         <v>650</v>
       </c>
-      <c r="R5" t="s">
+      <c r="T5" t="s">
         <v>59</v>
       </c>
-      <c r="T5" t="s">
+      <c r="V5" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="6" spans="2:26">
+    <row r="6" spans="2:28">
       <c r="B6">
         <v>2011</v>
       </c>
       <c r="C6" s="42">
         <v>15000</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="D6" s="42">
+        <f t="shared" si="0"/>
+        <v>2500</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="S6" t="s">
         <v>652</v>
       </c>
-      <c r="R6" t="s">
+      <c r="T6" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="7" spans="2:26">
+    <row r="7" spans="2:28">
       <c r="B7">
         <v>2012</v>
       </c>
       <c r="C7" s="42">
         <v>18000</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="D7" s="42">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="S7" t="s">
         <v>652</v>
       </c>
-      <c r="R7" t="s">
+      <c r="T7" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="8" spans="2:26">
+    <row r="8" spans="2:28">
       <c r="B8">
         <v>2013</v>
       </c>
       <c r="C8" s="42">
         <v>19000</v>
       </c>
-      <c r="R8" t="s">
+      <c r="D8" s="42">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>5.5555555555555554</v>
+      </c>
+      <c r="T8" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="9" spans="2:26">
+    <row r="9" spans="2:28">
       <c r="B9">
         <v>2014</v>
       </c>
       <c r="C9" s="42">
         <v>21000</v>
       </c>
-      <c r="R9" t="s">
+      <c r="D9" s="42">
+        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>10.526315789473683</v>
+      </c>
+      <c r="T9" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="10" spans="2:26">
+    <row r="10" spans="2:28">
       <c r="B10">
         <v>2015</v>
       </c>
       <c r="C10">
         <v>22802.21</v>
       </c>
-      <c r="R10" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="11" spans="2:26">
+      <c r="D10" s="42">
+        <f t="shared" si="0"/>
+        <v>1802.2099999999991</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>8.5819523809523766</v>
+      </c>
+      <c r="T10" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="11" spans="2:28">
       <c r="B11">
         <v>2016</v>
       </c>
       <c r="C11">
         <v>24571.22</v>
       </c>
-      <c r="R11" t="s">
+      <c r="D11" s="42">
+        <f t="shared" si="0"/>
+        <v>1769.010000000002</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>7.758063801710458</v>
+      </c>
+      <c r="T11" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="12" spans="2:26">
+    <row r="12" spans="2:28">
       <c r="B12">
         <v>2017</v>
       </c>
       <c r="C12">
         <v>31519.33</v>
       </c>
-      <c r="R12" t="s">
+      <c r="D12" s="42">
+        <f t="shared" si="0"/>
+        <v>6948.1100000000006</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>28.277431889828836</v>
+      </c>
+      <c r="T12" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="13" spans="2:26">
+    <row r="13" spans="2:28">
       <c r="B13">
         <v>2018</v>
       </c>
       <c r="C13">
         <v>36617.354169999999</v>
       </c>
-      <c r="R13" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="14" spans="2:26">
+      <c r="D13" s="42">
+        <f t="shared" si="0"/>
+        <v>5098.024169999997</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>16.174278355536099</v>
+      </c>
+      <c r="T13" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="14" spans="2:28">
       <c r="B14">
         <v>2019</v>
       </c>
       <c r="C14">
         <v>42465.77</v>
       </c>
-      <c r="R14" t="s">
+      <c r="D14" s="42">
+        <f t="shared" si="0"/>
+        <v>5848.4158299999981</v>
+      </c>
+      <c r="E14">
+        <f>D14/C13*100</f>
+        <v>15.971705117874164</v>
+      </c>
+      <c r="T14" t="s">
         <v>661</v>
       </c>
-      <c r="W14" t="s">
+      <c r="Y14" t="s">
         <v>32</v>
       </c>
-      <c r="X14" t="s">
+      <c r="Z14" t="s">
         <v>636</v>
       </c>
-      <c r="Y14" t="s">
+      <c r="AA14" t="s">
         <v>34</v>
       </c>
-      <c r="Z14" t="s">
+      <c r="AB14" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="2:26">
+    <row r="15" spans="2:28">
       <c r="B15">
         <v>2020</v>
       </c>
       <c r="C15">
         <v>43178.75</v>
       </c>
-      <c r="R15" t="s">
-        <v>677</v>
-      </c>
-      <c r="W15">
+      <c r="D15" s="42">
+        <f t="shared" si="0"/>
+        <v>712.9800000000032</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>1.6789522478928398</v>
+      </c>
+      <c r="T15" t="s">
+        <v>675</v>
+      </c>
+      <c r="Y15">
         <v>1400</v>
       </c>
-      <c r="X15">
+      <c r="Z15">
         <v>1650</v>
       </c>
-      <c r="Y15">
+      <c r="AA15">
         <v>1900</v>
       </c>
-      <c r="Z15">
+      <c r="AB15">
         <v>2150</v>
       </c>
     </row>
-    <row r="16" spans="2:26">
+    <row r="16" spans="2:28">
       <c r="B16">
         <v>2021</v>
       </c>
       <c r="C16">
         <v>45893.11</v>
       </c>
-    </row>
-    <row r="17" spans="2:27">
+      <c r="D16" s="42">
+        <f t="shared" si="0"/>
+        <v>2714.3600000000006</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>6.2863329762904225</v>
+      </c>
+    </row>
+    <row r="17" spans="2:29">
       <c r="B17">
         <v>2022</v>
       </c>
       <c r="C17">
         <v>48929.4</v>
       </c>
-    </row>
-    <row r="18" spans="2:27">
+      <c r="D17" s="42">
+        <f t="shared" si="0"/>
+        <v>3036.2900000000009</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>6.6160040145459762</v>
+      </c>
+    </row>
+    <row r="18" spans="2:29">
       <c r="B18">
         <v>2023</v>
       </c>
       <c r="C18" s="24">
         <v>52201.22</v>
       </c>
-    </row>
-    <row r="19" spans="2:27">
+      <c r="D18" s="24">
+        <f t="shared" si="0"/>
+        <v>3271.8199999999997</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>6.6868181502327833</v>
+      </c>
+    </row>
+    <row r="19" spans="2:29">
       <c r="B19">
         <v>2024</v>
       </c>
       <c r="C19" s="42">
         <v>55855.31</v>
       </c>
-    </row>
-    <row r="20" spans="2:27">
+      <c r="D19" s="42"/>
+    </row>
+    <row r="20" spans="2:29">
       <c r="B20">
         <v>2025</v>
       </c>
       <c r="C20" s="42">
         <v>59765.18</v>
       </c>
-    </row>
-    <row r="21" spans="2:27">
+      <c r="D20" s="42"/>
+    </row>
+    <row r="21" spans="2:29">
       <c r="B21">
         <v>2026</v>
       </c>
       <c r="C21" s="42">
         <v>63948.74</v>
       </c>
-    </row>
-    <row r="22" spans="2:27">
+      <c r="D21" s="42"/>
+    </row>
+    <row r="22" spans="2:29">
       <c r="B22">
         <v>2027</v>
       </c>
       <c r="C22" s="42">
         <v>68425.149999999994</v>
       </c>
-      <c r="W22" s="26" t="s">
+      <c r="D22" s="42"/>
+      <c r="Y22" s="26" t="s">
         <v>621</v>
       </c>
-      <c r="X22" s="255" t="s">
+      <c r="Z22" s="255" t="s">
         <v>667</v>
       </c>
-      <c r="Y22" s="255"/>
-      <c r="Z22" s="255"/>
-      <c r="AA22" t="s">
+      <c r="AA22" s="255"/>
+      <c r="AB22" s="255"/>
+      <c r="AC22" t="s">
         <v>668</v>
       </c>
     </row>
-    <row r="23" spans="2:27">
+    <row r="23" spans="2:29">
       <c r="B23">
         <v>2028</v>
       </c>
       <c r="C23" s="42">
         <v>73214.91</v>
       </c>
-      <c r="W23" t="s">
+      <c r="D23" s="42"/>
+      <c r="Y23" t="s">
         <v>410</v>
       </c>
-      <c r="X23" t="s">
+      <c r="Z23" t="s">
         <v>618</v>
       </c>
-      <c r="Y23" t="s">
+      <c r="AA23" t="s">
         <v>619</v>
       </c>
-      <c r="Z23" t="s">
+      <c r="AB23" t="s">
         <v>622</v>
       </c>
     </row>
-    <row r="24" spans="2:27" ht="23.25">
-      <c r="B24" s="253" t="s">
+    <row r="24" spans="2:29">
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="N24" s="254" t="s">
+        <v>606</v>
+      </c>
+      <c r="O24" s="254"/>
+      <c r="P24" s="254"/>
+      <c r="T24" s="243" t="s">
+        <v>613</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>50</v>
+      </c>
+      <c r="Z24">
+        <v>200</v>
+      </c>
+      <c r="AA24">
+        <f>Z24+(Y24*12)</f>
+        <v>800</v>
+      </c>
+    </row>
+    <row r="25" spans="2:29" ht="23.25">
+      <c r="B25" s="253" t="s">
         <v>602</v>
       </c>
-      <c r="C24" s="253"/>
-      <c r="D24" s="253"/>
-      <c r="E24" s="253"/>
-      <c r="F24" s="253"/>
-      <c r="M24" s="254" t="s">
-        <v>606</v>
-      </c>
-      <c r="N24" s="254"/>
-      <c r="O24" s="254"/>
-      <c r="S24" s="243" t="s">
-        <v>613</v>
-      </c>
-      <c r="W24">
-        <v>0</v>
-      </c>
-      <c r="X24">
-        <v>50</v>
-      </c>
-      <c r="Y24">
-        <v>200</v>
-      </c>
-      <c r="Z24">
-        <f>Y24+(X24*12)</f>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="25" spans="2:27">
-      <c r="C25" s="180" t="s">
+      <c r="C25" s="253"/>
+      <c r="D25" s="253"/>
+      <c r="E25" s="253"/>
+      <c r="F25" s="253"/>
+      <c r="N25">
+        <v>52201.22</v>
+      </c>
+      <c r="O25" s="180" t="s">
+        <v>236</v>
+      </c>
+      <c r="U25" t="s">
+        <v>615</v>
+      </c>
+      <c r="X25">
+        <v>1</v>
+      </c>
+      <c r="Y25">
+        <v>100</v>
+      </c>
+      <c r="Z25">
+        <v>5000</v>
+      </c>
+      <c r="AA25">
+        <f>Z25+(Y25*12)</f>
+        <v>6200</v>
+      </c>
+    </row>
+    <row r="26" spans="2:29">
+      <c r="C26" s="180" t="s">
         <v>600</v>
       </c>
-      <c r="D25" s="180" t="s">
+      <c r="D26" s="180" t="s">
         <v>597</v>
       </c>
-      <c r="E25" s="180" t="s">
+      <c r="E26" s="180" t="s">
         <v>603</v>
       </c>
-      <c r="M25">
-        <v>52201.22</v>
-      </c>
-      <c r="N25" s="180" t="s">
-        <v>236</v>
-      </c>
-      <c r="T25" t="s">
-        <v>615</v>
-      </c>
-      <c r="W25">
-        <v>1</v>
-      </c>
-      <c r="X25">
-        <v>100</v>
-      </c>
-      <c r="Y25">
-        <v>5000</v>
-      </c>
-      <c r="Z25">
-        <f>Y25+(X25*12)</f>
-        <v>6200</v>
-      </c>
-    </row>
-    <row r="26" spans="2:27">
-      <c r="D26" t="s">
+      <c r="N26">
+        <f>N25*0.3</f>
+        <v>15660.366</v>
+      </c>
+      <c r="O26" t="s">
+        <v>607</v>
+      </c>
+      <c r="T26">
+        <v>20332.669999999998</v>
+      </c>
+      <c r="U26">
+        <f>T26/N25*100</f>
+        <v>38.950564756915639</v>
+      </c>
+      <c r="X26">
+        <v>2</v>
+      </c>
+      <c r="Y26">
+        <v>350</v>
+      </c>
+      <c r="Z26">
+        <v>1000</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" ref="AA26:AA31" si="2">AA25+Z26++(Y26*12)</f>
+        <v>11400</v>
+      </c>
+    </row>
+    <row r="27" spans="2:29">
+      <c r="D27" t="s">
         <v>596</v>
       </c>
-      <c r="E26" t="s">
+      <c r="E27" t="s">
         <v>598</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F27" t="s">
         <v>599</v>
       </c>
-      <c r="M26">
-        <f>M25*0.3</f>
-        <v>15660.366</v>
-      </c>
-      <c r="N26" t="s">
-        <v>607</v>
-      </c>
-      <c r="S26">
-        <v>20332.669999999998</v>
-      </c>
-      <c r="T26">
-        <f>S26/M25*100</f>
-        <v>38.950564756915639</v>
-      </c>
-      <c r="W26">
-        <v>2</v>
-      </c>
-      <c r="X26">
-        <v>350</v>
-      </c>
-      <c r="Y26">
+      <c r="N27">
+        <f>N25*0.15</f>
+        <v>7830.183</v>
+      </c>
+      <c r="O27" t="s">
+        <v>608</v>
+      </c>
+      <c r="T27">
+        <v>7000</v>
+      </c>
+      <c r="U27">
+        <f>T27/N25*100</f>
+        <v>13.409648280250922</v>
+      </c>
+      <c r="X27">
+        <v>3</v>
+      </c>
+      <c r="Y27">
+        <v>500</v>
+      </c>
+      <c r="Z27">
         <v>1000</v>
       </c>
-      <c r="Z26">
-        <f t="shared" ref="Z26:Z31" si="0">Z25+Y26++(X26*12)</f>
-        <v>11400</v>
-      </c>
-    </row>
-    <row r="27" spans="2:27">
-      <c r="B27" s="242">
+      <c r="AA27">
+        <f t="shared" si="2"/>
+        <v>18400</v>
+      </c>
+    </row>
+    <row r="28" spans="2:29">
+      <c r="B28" s="242">
         <v>44835</v>
       </c>
-      <c r="C27">
+      <c r="C28">
         <v>75000</v>
       </c>
-      <c r="D27">
+      <c r="D28">
         <v>1000</v>
       </c>
-      <c r="E27">
-        <f t="shared" ref="E27:E32" si="1">C27/D27</f>
+      <c r="E28">
+        <f t="shared" ref="E28:E33" si="3">C28/D28</f>
         <v>75</v>
       </c>
-      <c r="F27">
-        <f t="shared" ref="F27:F32" si="2">ROUNDUP(E27/12,1)</f>
+      <c r="F28">
+        <f t="shared" ref="F28:F33" si="4">ROUNDUP(E28/12,1)</f>
         <v>6.3</v>
       </c>
-      <c r="M27">
-        <f>M25*0.15</f>
+      <c r="N28">
+        <f>N25*0.15</f>
         <v>7830.183</v>
       </c>
-      <c r="N27" t="s">
-        <v>608</v>
-      </c>
-      <c r="S27">
-        <v>7000</v>
-      </c>
-      <c r="T27">
-        <f>S27/M25*100</f>
-        <v>13.409648280250922</v>
-      </c>
-      <c r="W27">
-        <v>3</v>
-      </c>
-      <c r="X27">
-        <v>500</v>
-      </c>
-      <c r="Y27">
-        <v>1000</v>
-      </c>
-      <c r="Z27">
-        <f t="shared" si="0"/>
-        <v>18400</v>
-      </c>
-    </row>
-    <row r="28" spans="2:27">
-      <c r="B28" s="242">
-        <v>44866</v>
-      </c>
-      <c r="C28">
-        <v>74000</v>
-      </c>
-      <c r="D28">
-        <v>3500</v>
-      </c>
-      <c r="E28">
-        <f t="shared" si="1"/>
-        <v>21.142857142857142</v>
-      </c>
-      <c r="F28">
-        <f t="shared" si="2"/>
-        <v>1.8</v>
-      </c>
-      <c r="M28">
-        <f>M25*0.15</f>
-        <v>7830.183</v>
-      </c>
-      <c r="N28" t="s">
+      <c r="O28" t="s">
         <v>609</v>
       </c>
-      <c r="S28">
+      <c r="T28">
         <f>2800</f>
         <v>2800</v>
       </c>
-      <c r="T28">
-        <f>S28/M25*100</f>
+      <c r="U28">
+        <f>T28/N25*100</f>
         <v>5.3638593121003684</v>
       </c>
-      <c r="W28">
+      <c r="X28">
         <v>4</v>
       </c>
-      <c r="X28">
+      <c r="Y28">
         <v>350</v>
       </c>
-      <c r="Y28">
+      <c r="Z28">
         <v>1000</v>
       </c>
-      <c r="Z28">
-        <f t="shared" si="0"/>
+      <c r="AA28">
+        <f t="shared" si="2"/>
         <v>23600</v>
       </c>
     </row>
-    <row r="29" spans="2:27">
+    <row r="29" spans="2:29">
       <c r="B29" s="242">
-        <v>44896</v>
-      </c>
-      <c r="C29" s="244">
-        <v>66000</v>
+        <v>44866</v>
+      </c>
+      <c r="C29">
+        <v>74000</v>
       </c>
       <c r="D29">
-        <v>3000</v>
+        <v>3500</v>
       </c>
       <c r="E29">
-        <f t="shared" si="1"/>
-        <v>22</v>
+        <f t="shared" si="3"/>
+        <v>21.142857142857142</v>
       </c>
       <c r="F29">
-        <f t="shared" si="2"/>
-        <v>1.9000000000000001</v>
+        <f t="shared" si="4"/>
+        <v>1.8</v>
       </c>
       <c r="G29" s="244" t="s">
         <v>623</v>
       </c>
-      <c r="M29">
-        <f>M25*0.2</f>
+      <c r="N29">
+        <f>N25*0.2</f>
         <v>10440.244000000001</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>610</v>
       </c>
-      <c r="S29">
+      <c r="T29">
         <f>754.37+312.8+2139.86</f>
         <v>3207.03</v>
       </c>
-      <c r="T29">
-        <f>S29/M25*100</f>
+      <c r="U29">
+        <f>T29/N25*100</f>
         <v>6.1435920463161589</v>
       </c>
-      <c r="W29">
+      <c r="X29">
         <v>5</v>
       </c>
-      <c r="X29">
+      <c r="Y29">
         <v>350</v>
       </c>
-      <c r="Y29">
+      <c r="Z29">
         <v>1000</v>
       </c>
-      <c r="Z29">
-        <f t="shared" si="0"/>
+      <c r="AA29">
+        <f t="shared" si="2"/>
         <v>28800</v>
       </c>
     </row>
-    <row r="30" spans="2:27">
+    <row r="30" spans="2:29">
       <c r="B30" s="242">
-        <v>44927</v>
+        <v>44896</v>
       </c>
       <c r="C30" s="244">
-        <v>71000</v>
+        <v>66000</v>
       </c>
       <c r="D30">
         <v>3000</v>
       </c>
       <c r="E30">
-        <f t="shared" si="1"/>
-        <v>23.666666666666668</v>
+        <f t="shared" si="3"/>
+        <v>22</v>
       </c>
       <c r="F30">
+        <f t="shared" si="4"/>
+        <v>1.9000000000000001</v>
+      </c>
+      <c r="N30">
+        <f>N25*0.1</f>
+        <v>5220.1220000000003</v>
+      </c>
+      <c r="O30" t="s">
+        <v>611</v>
+      </c>
+      <c r="T30">
+        <v>3500</v>
+      </c>
+      <c r="U30">
+        <f>T30/N25*100</f>
+        <v>6.7048241401254609</v>
+      </c>
+      <c r="X30">
+        <v>6</v>
+      </c>
+      <c r="Y30">
+        <v>350</v>
+      </c>
+      <c r="Z30">
+        <v>1000</v>
+      </c>
+      <c r="AA30">
         <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="M30">
-        <f>M25*0.1</f>
-        <v>5220.1220000000003</v>
-      </c>
-      <c r="N30" t="s">
-        <v>611</v>
-      </c>
-      <c r="S30">
-        <v>3500</v>
-      </c>
-      <c r="T30">
-        <f>S30/M25*100</f>
-        <v>6.7048241401254609</v>
-      </c>
-      <c r="W30">
-        <v>6</v>
-      </c>
-      <c r="X30">
-        <v>350</v>
-      </c>
-      <c r="Y30">
-        <v>1000</v>
-      </c>
-      <c r="Z30">
-        <f t="shared" si="0"/>
         <v>34000</v>
       </c>
     </row>
-    <row r="31" spans="2:27">
+    <row r="31" spans="2:29">
       <c r="B31" s="242">
-        <v>44958</v>
-      </c>
-      <c r="C31">
-        <v>74000</v>
+        <v>44927</v>
+      </c>
+      <c r="C31" s="244">
+        <v>71000</v>
       </c>
       <c r="D31">
         <v>3000</v>
       </c>
       <c r="E31">
-        <f t="shared" si="1"/>
-        <v>24.666666666666668</v>
+        <f t="shared" si="3"/>
+        <v>23.666666666666668</v>
       </c>
       <c r="F31">
-        <f t="shared" si="2"/>
-        <v>2.1</v>
-      </c>
-      <c r="M31">
-        <f>M25*0.05</f>
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="N31">
+        <f>N25*0.05</f>
         <v>2610.0610000000001</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>612</v>
       </c>
-      <c r="S31">
+      <c r="T31">
         <f>727+159+1000</f>
         <v>1886</v>
       </c>
-      <c r="T31">
-        <f>S31/M25*100</f>
+      <c r="U31">
+        <f>T31/N25*100</f>
         <v>3.6129423795076052</v>
       </c>
-      <c r="W31">
+      <c r="X31">
         <v>7</v>
       </c>
-      <c r="X31">
+      <c r="Y31">
         <v>350</v>
       </c>
-      <c r="Y31">
+      <c r="Z31">
         <v>1000</v>
       </c>
-      <c r="Z31">
-        <f t="shared" si="0"/>
+      <c r="AA31">
+        <f t="shared" si="2"/>
         <v>39200</v>
       </c>
     </row>
-    <row r="32" spans="2:27">
+    <row r="32" spans="2:29">
       <c r="B32" s="242">
-        <v>44986</v>
+        <v>44958</v>
       </c>
       <c r="C32">
-        <v>0</v>
+        <v>74000</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>3000</v>
       </c>
       <c r="E32">
-        <f t="shared" si="1"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>24.666666666666668</v>
       </c>
       <c r="F32">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>2.1</v>
       </c>
       <c r="G32" t="s">
         <v>627</v>
       </c>
-      <c r="M32">
-        <f>M25*0.05</f>
+      <c r="N32">
+        <f>N25*0.05</f>
         <v>2610.0610000000001</v>
       </c>
-      <c r="N32" t="s">
+      <c r="O32" t="s">
         <v>614</v>
       </c>
-      <c r="S32">
+      <c r="T32">
         <f>4000+495+3080</f>
         <v>7575</v>
       </c>
-      <c r="T32">
-        <f>S32/M25*100</f>
+      <c r="U32">
+        <f>T32/N25*100</f>
         <v>14.511155103271534</v>
       </c>
-      <c r="W32">
+      <c r="X32">
         <v>8</v>
       </c>
-      <c r="X32">
+      <c r="Y32">
         <v>350</v>
       </c>
-      <c r="Y32">
+      <c r="Z32">
         <v>1000</v>
       </c>
-      <c r="Z32">
-        <f t="shared" ref="Z32:Z33" si="3">Z31+Y32++(X32*12)</f>
+      <c r="AA32">
+        <f t="shared" ref="AA32:AA33" si="5">AA31+Z32++(Y32*12)</f>
         <v>44400</v>
       </c>
     </row>
-    <row r="33" spans="2:26">
+    <row r="33" spans="2:27">
+      <c r="B33" s="242">
+        <v>44986</v>
+      </c>
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
       <c r="G33" s="126">
         <v>74000</v>
       </c>
-      <c r="S33" s="180" t="s">
+      <c r="T33" s="180" t="s">
         <v>159</v>
       </c>
-      <c r="T33">
-        <f>M25-SUM(S26:S32)</f>
+      <c r="U33">
+        <f>N25-SUM(T26:T32)</f>
         <v>5900.5200000000041</v>
       </c>
-      <c r="W33">
+      <c r="X33">
         <v>9</v>
       </c>
-      <c r="X33">
+      <c r="Y33">
         <v>350</v>
       </c>
-      <c r="Y33">
+      <c r="Z33">
         <v>1000</v>
       </c>
-      <c r="Z33">
-        <f t="shared" si="3"/>
+      <c r="AA33">
+        <f t="shared" si="5"/>
         <v>49600</v>
       </c>
     </row>
-    <row r="34" spans="2:26">
-      <c r="W34">
+    <row r="34" spans="2:27">
+      <c r="X34">
         <v>10</v>
       </c>
-      <c r="X34">
+      <c r="Y34">
         <v>350</v>
       </c>
-      <c r="Y34">
+      <c r="Z34">
         <v>1000</v>
       </c>
-      <c r="Z34">
-        <f t="shared" ref="Z34" si="4">Z33+Y34++(X34*12)</f>
+      <c r="AA34">
+        <f t="shared" ref="AA34" si="6">AA33+Z34++(Y34*12)</f>
         <v>54800</v>
       </c>
     </row>
-    <row r="35" spans="2:26">
-      <c r="F35">
+    <row r="36" spans="2:27">
+      <c r="F36">
         <f>48929.4*1.07</f>
         <v>52354.458000000006</v>
       </c>
     </row>
-    <row r="37" spans="2:26">
-      <c r="C37" s="169" t="s">
+    <row r="38" spans="2:27">
+      <c r="C38" s="169" t="s">
         <v>643</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D38" t="s">
         <v>628</v>
       </c>
     </row>
-    <row r="38" spans="2:26">
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" t="s">
+    <row r="39" spans="2:27">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" t="s">
         <v>629</v>
       </c>
     </row>
-    <row r="39" spans="2:26">
-      <c r="C39">
+    <row r="40" spans="2:27">
+      <c r="C40">
         <v>14</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D40" t="s">
         <v>630</v>
       </c>
     </row>
-    <row r="40" spans="2:26">
-      <c r="C40">
+    <row r="41" spans="2:27">
+      <c r="C41">
         <v>85</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>631</v>
       </c>
     </row>
-    <row r="42" spans="2:26">
-      <c r="D42" t="s">
-        <v>678</v>
-      </c>
+    <row r="42" spans="2:27">
       <c r="G42" t="s">
-        <v>679</v>
-      </c>
-    </row>
-    <row r="43" spans="2:26">
-      <c r="D43">
-        <f>SUM(C46:C1048576)</f>
+        <v>677</v>
+      </c>
+    </row>
+    <row r="43" spans="2:27">
+      <c r="D43" t="s">
+        <v>676</v>
+      </c>
+      <c r="G43">
+        <f>SUM(E47:E1048576)</f>
+        <v>7609.3099999999995</v>
+      </c>
+    </row>
+    <row r="44" spans="2:27">
+      <c r="D44">
+        <f>SUM(C47:C1048576)</f>
         <v>9606.69</v>
       </c>
-      <c r="G43">
-        <f>SUM(E46:E1048576)</f>
-        <v>4425.3899999999994</v>
-      </c>
-    </row>
-    <row r="44" spans="2:26">
-      <c r="B44" t="s">
+    </row>
+    <row r="45" spans="2:27">
+      <c r="B45" t="s">
         <v>637</v>
       </c>
-      <c r="D44">
-        <f>SUM(C46:C1000)</f>
+      <c r="D45">
+        <f>SUM(C47:C1002)</f>
         <v>9606.69</v>
       </c>
     </row>
-    <row r="45" spans="2:26">
-      <c r="C45" t="s">
+    <row r="46" spans="2:27" ht="15.75" thickBot="1">
+      <c r="C46" t="s">
         <v>644</v>
       </c>
-      <c r="E45" t="s">
+      <c r="E46" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="46" spans="2:26" ht="15.75" thickBot="1">
-      <c r="B46" t="s">
-        <v>638</v>
-      </c>
-      <c r="C46">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="47" spans="2:26" ht="16.5" thickTop="1" thickBot="1">
+    <row r="47" spans="2:27" ht="16.5" thickTop="1" thickBot="1">
       <c r="B47" t="s">
         <v>638</v>
       </c>
       <c r="C47">
+        <v>500</v>
+      </c>
+      <c r="H47" s="118" t="s">
+        <v>678</v>
+      </c>
+      <c r="I47" s="118" t="s">
+        <v>679</v>
+      </c>
+      <c r="J47" s="118" t="s">
+        <v>691</v>
+      </c>
+      <c r="M47" s="118" t="s">
+        <v>680</v>
+      </c>
+      <c r="N47" s="118" t="s">
+        <v>681</v>
+      </c>
+      <c r="O47" s="118" t="s">
+        <v>682</v>
+      </c>
+      <c r="P47" s="118" t="s">
+        <v>695</v>
+      </c>
+      <c r="Q47" s="118" t="s">
+        <v>685</v>
+      </c>
+      <c r="R47" s="118" t="s">
+        <v>684</v>
+      </c>
+      <c r="S47" s="118" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="48" spans="2:27" ht="16.5" thickTop="1" thickBot="1">
+      <c r="B48" t="s">
+        <v>638</v>
+      </c>
+      <c r="C48">
         <v>1500</v>
       </c>
-      <c r="H47" s="118" t="s">
-        <v>680</v>
-      </c>
-      <c r="I47" s="118" t="s">
-        <v>681</v>
-      </c>
-      <c r="J47" s="118"/>
-      <c r="K47" s="118" t="s">
-        <v>682</v>
-      </c>
-      <c r="L47" s="118" t="s">
-        <v>683</v>
-      </c>
-      <c r="M47" s="118" t="s">
-        <v>684</v>
-      </c>
-      <c r="N47" s="118" t="s">
+      <c r="G48" s="118" t="s">
         <v>687</v>
       </c>
-      <c r="O47" s="118" t="s">
-        <v>686</v>
-      </c>
-      <c r="P47" s="118" t="s">
+      <c r="H48">
+        <f>E49+E60</f>
+        <v>964.79</v>
+      </c>
+      <c r="I48">
+        <f>E51+E59</f>
+        <v>2109.56</v>
+      </c>
+      <c r="J48">
+        <v>1423.51</v>
+      </c>
+      <c r="K48">
+        <f>SUM(H48:J48)</f>
+        <v>4497.8599999999997</v>
+      </c>
+      <c r="L48">
+        <f>SUM(M48:P48)</f>
+        <v>3101.79</v>
+      </c>
+      <c r="M48">
+        <f>E52</f>
+        <v>431.52000000000004</v>
+      </c>
+      <c r="N48">
+        <f>E56</f>
+        <v>534.66</v>
+      </c>
+      <c r="O48">
+        <f>E53</f>
+        <v>375.20000000000005</v>
+      </c>
+      <c r="P48">
+        <v>1760.41</v>
+      </c>
+      <c r="S48" s="42" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="48" spans="2:26" ht="16.5" thickTop="1" thickBot="1">
-      <c r="B48" s="250">
+    <row r="49" spans="2:20" ht="15.75" thickTop="1">
+      <c r="B49" s="250">
         <v>45050</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D49" s="16" t="s">
         <v>639</v>
       </c>
-      <c r="E48">
+      <c r="E49">
         <f>40*11.56</f>
         <v>462.40000000000003</v>
       </c>
-      <c r="G48" s="118" t="s">
-        <v>689</v>
-      </c>
-      <c r="H48">
-        <f>E48+E59</f>
-        <v>964.79</v>
-      </c>
-      <c r="I48">
-        <f>E50+E58</f>
-        <v>2109.56</v>
-      </c>
-      <c r="K48">
-        <f>E51</f>
-        <v>431.52000000000004</v>
-      </c>
-      <c r="L48">
-        <f>E55</f>
-        <v>534.66</v>
-      </c>
-      <c r="M48">
-        <f>E52</f>
-        <v>375.20000000000005</v>
-      </c>
-      <c r="P48" s="42" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="49" spans="2:17" ht="15.75" thickTop="1">
-      <c r="B49" s="250">
-        <v>45050</v>
-      </c>
-      <c r="C49">
-        <v>500</v>
-      </c>
       <c r="G49" s="250">
         <v>45223</v>
       </c>
@@ -6516,32 +6693,39 @@
       <c r="I49">
         <v>2008</v>
       </c>
+      <c r="J49">
+        <v>1423.51</v>
+      </c>
       <c r="K49">
+        <f>SUM(H49:J49)</f>
+        <v>4375.51</v>
+      </c>
+      <c r="L49">
+        <f>SUM(M49:P49)</f>
+        <v>1319</v>
+      </c>
+      <c r="M49">
         <v>459</v>
       </c>
-      <c r="L49">
+      <c r="N49">
         <v>501</v>
       </c>
-      <c r="M49">
+      <c r="O49">
         <v>359</v>
       </c>
-      <c r="P49" s="24" t="s">
-        <v>691</v>
-      </c>
-    </row>
-    <row r="50" spans="2:17">
+      <c r="S49" s="24" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="50" spans="2:20">
       <c r="B50" s="250">
-        <v>45054</v>
-      </c>
-      <c r="D50" s="16" t="s">
-        <v>640</v>
-      </c>
-      <c r="E50">
-        <f>10*103.4</f>
-        <v>1034</v>
+        <v>45050</v>
+      </c>
+      <c r="C50">
+        <v>500</v>
       </c>
       <c r="G50" s="20" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="H50">
         <f>H48-H49</f>
@@ -6551,167 +6735,289 @@
         <f>I48-I49</f>
         <v>101.55999999999995</v>
       </c>
-      <c r="K50">
-        <f>K48-K49</f>
-        <v>-27.479999999999961</v>
-      </c>
-      <c r="L50">
-        <f>L48-L49</f>
-        <v>33.659999999999968</v>
+      <c r="J50">
+        <f>J48-J49</f>
+        <v>0</v>
       </c>
       <c r="M50">
         <f>M48-M49</f>
+        <v>-27.479999999999961</v>
+      </c>
+      <c r="N50">
+        <f>N48-N49</f>
+        <v>33.659999999999968</v>
+      </c>
+      <c r="O50">
+        <f>O48-O49</f>
         <v>16.200000000000045</v>
       </c>
-      <c r="N50">
-        <f>SUMIF(H50:M50,"&lt;0")</f>
-        <v>-27.479999999999961</v>
-      </c>
-      <c r="O50">
-        <f>SUMIF(I50:N50,"&gt;0")</f>
-        <v>151.41999999999996</v>
-      </c>
-      <c r="P50">
-        <f>(O50+N50)*-1</f>
-        <v>-123.94</v>
-      </c>
-      <c r="Q50" s="250">
+      <c r="Q50">
+        <f>SUMIF(H50:O50,"&lt;0")*-1</f>
+        <v>27.479999999999961</v>
+      </c>
+      <c r="R50">
+        <f>SUMIF(I50:Q50,"&gt;0")</f>
+        <v>178.89999999999992</v>
+      </c>
+      <c r="S50">
+        <f>(Q50-R50)</f>
+        <v>-151.41999999999996</v>
+      </c>
+      <c r="T50" s="250">
         <v>45223</v>
       </c>
     </row>
-    <row r="51" spans="2:17">
+    <row r="51" spans="2:20">
       <c r="B51" s="250">
+        <v>45054</v>
+      </c>
+      <c r="D51" s="16" t="s">
+        <v>640</v>
+      </c>
+      <c r="E51">
+        <f>10*103.4</f>
+        <v>1034</v>
+      </c>
+      <c r="S51" s="42" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="52" spans="2:20">
+      <c r="B52" s="250">
         <v>45055</v>
       </c>
-      <c r="D51" s="252" t="s">
+      <c r="D52" s="252" t="s">
         <v>641</v>
       </c>
-      <c r="E51">
+      <c r="E52">
         <f>29*14.88</f>
         <v>431.52000000000004</v>
       </c>
-    </row>
-    <row r="52" spans="2:17">
-      <c r="B52" s="250">
+      <c r="G52" s="250">
+        <v>45255</v>
+      </c>
+      <c r="H52">
+        <v>972</v>
+      </c>
+      <c r="I52">
+        <v>2116</v>
+      </c>
+      <c r="J52">
+        <v>1621</v>
+      </c>
+      <c r="K52">
+        <f>SUM(H52:J52)</f>
+        <v>4709</v>
+      </c>
+      <c r="L52">
+        <f>SUM(M52:P52)</f>
+        <v>3205</v>
+      </c>
+      <c r="M52">
+        <v>504</v>
+      </c>
+      <c r="N52">
+        <v>561</v>
+      </c>
+      <c r="O52">
+        <v>393</v>
+      </c>
+      <c r="P52">
+        <v>1747</v>
+      </c>
+      <c r="S52" s="24" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="53" spans="2:20">
+      <c r="B53" s="250">
         <v>45085</v>
       </c>
-      <c r="D52" s="252" t="s">
+      <c r="D53" s="252" t="s">
         <v>642</v>
       </c>
-      <c r="E52">
+      <c r="E53">
         <f>40*9.38</f>
         <v>375.20000000000005</v>
       </c>
-    </row>
-    <row r="53" spans="2:17">
-      <c r="B53" s="250">
+      <c r="G53" s="20" t="s">
+        <v>683</v>
+      </c>
+      <c r="H53">
+        <f>H48-H52</f>
+        <v>-7.2100000000000364</v>
+      </c>
+      <c r="I53">
+        <f>I48-I52</f>
+        <v>-6.4400000000000546</v>
+      </c>
+      <c r="J53">
+        <f>J48-J52</f>
+        <v>-197.49</v>
+      </c>
+      <c r="M53">
+        <f>M48-M52</f>
+        <v>-72.479999999999961</v>
+      </c>
+      <c r="N53">
+        <f>N48-N52</f>
+        <v>-26.340000000000032</v>
+      </c>
+      <c r="O53">
+        <f>O48-O52</f>
+        <v>-17.799999999999955</v>
+      </c>
+      <c r="P53">
+        <f>P48-P52</f>
+        <v>13.410000000000082</v>
+      </c>
+      <c r="Q53">
+        <f>SUMIF(H53:O53,"&lt;0")</f>
+        <v>-327.76000000000005</v>
+      </c>
+      <c r="R53">
+        <f>SUMIF(I53:Q53,"&gt;0")</f>
+        <v>13.410000000000082</v>
+      </c>
+      <c r="S53">
+        <f>(R53+Q53)*-1</f>
+        <v>314.34999999999997</v>
+      </c>
+      <c r="T53" s="250">
+        <v>45257</v>
+      </c>
+    </row>
+    <row r="54" spans="2:20">
+      <c r="B54" s="250">
         <v>45110</v>
       </c>
-      <c r="C53">
+      <c r="C54">
         <v>500</v>
       </c>
     </row>
-    <row r="54" spans="2:17">
-      <c r="B54" s="250">
-        <v>45113</v>
-      </c>
-      <c r="D54" s="44" t="s">
-        <v>662</v>
-      </c>
-      <c r="E54">
-        <v>9.66</v>
-      </c>
-    </row>
-    <row r="55" spans="2:17">
+    <row r="55" spans="2:20">
       <c r="B55" s="250">
         <v>45113</v>
       </c>
-      <c r="C55">
+      <c r="D55" s="44" t="s">
+        <v>662</v>
+      </c>
+      <c r="E55">
+        <v>9.66</v>
+      </c>
+    </row>
+    <row r="56" spans="2:20">
+      <c r="B56" s="250">
+        <v>45113</v>
+      </c>
+      <c r="C56">
         <v>525</v>
       </c>
-      <c r="D55" s="252" t="s">
+      <c r="D56" s="252" t="s">
         <v>663</v>
       </c>
-      <c r="E55">
+      <c r="E56">
         <v>534.66</v>
       </c>
     </row>
-    <row r="56" spans="2:17">
-      <c r="B56" s="250">
+    <row r="57" spans="2:20">
+      <c r="B57" s="250">
         <v>45191</v>
       </c>
-      <c r="C56">
+      <c r="C57">
         <v>56.09</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D57" s="16" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="57" spans="2:17" ht="39">
-      <c r="B57" s="250">
-        <v>45215</v>
-      </c>
-      <c r="C57">
-        <v>5000</v>
-      </c>
-      <c r="D57" s="251" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="58" spans="2:17">
+    <row r="58" spans="2:20" ht="39">
       <c r="B58" s="250">
         <v>45215</v>
       </c>
-      <c r="D58" s="16" t="s">
-        <v>665</v>
-      </c>
-      <c r="E58">
-        <v>1075.56</v>
-      </c>
-    </row>
-    <row r="59" spans="2:17">
+      <c r="C58">
+        <v>5000</v>
+      </c>
+      <c r="D58" s="251" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="59" spans="2:20">
       <c r="B59" s="250">
         <v>45215</v>
       </c>
       <c r="D59" s="16" t="s">
+        <v>665</v>
+      </c>
+      <c r="E59">
+        <v>1075.56</v>
+      </c>
+    </row>
+    <row r="60" spans="2:20">
+      <c r="B60" s="250">
+        <v>45215</v>
+      </c>
+      <c r="D60" s="16" t="s">
         <v>666</v>
       </c>
-      <c r="E59">
+      <c r="E60">
         <v>502.39</v>
       </c>
     </row>
-    <row r="60" spans="2:17">
-      <c r="B60" s="250">
+    <row r="61" spans="2:20">
+      <c r="B61" s="250">
         <v>45222</v>
       </c>
-      <c r="C60">
+      <c r="C61">
         <v>25.6</v>
       </c>
-      <c r="D60" s="16" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="61" spans="2:17">
-      <c r="B61" s="250">
+      <c r="D61" s="16" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="62" spans="2:20">
+      <c r="B62" s="250">
         <v>45223</v>
-      </c>
-      <c r="C61">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="62" spans="2:17">
-      <c r="B62" s="250">
-        <v>45255</v>
       </c>
       <c r="C62">
         <v>500</v>
       </c>
     </row>
+    <row r="63" spans="2:20">
+      <c r="B63" s="250">
+        <v>45225</v>
+      </c>
+      <c r="D63" s="16" t="s">
+        <v>690</v>
+      </c>
+      <c r="E63">
+        <v>1423.51</v>
+      </c>
+    </row>
+    <row r="64" spans="2:20">
+      <c r="B64" s="250">
+        <v>45255</v>
+      </c>
+      <c r="C64">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="65" spans="2:5">
+      <c r="B65" s="250">
+        <v>45257</v>
+      </c>
+      <c r="D65" s="16" t="s">
+        <v>698</v>
+      </c>
+      <c r="E65">
+        <v>1760.41</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="M24:O24"/>
-    <mergeCell ref="X22:Z22"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="N24:P24"/>
+    <mergeCell ref="Z22:AB22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
@@ -19855,8 +20161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33331D36-B2E1-4FAB-B650-B9E2B082374C}">
   <dimension ref="A1:AF111"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="I4" sqref="H4:I4"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19961,7 +20267,7 @@
       </c>
       <c r="H2" s="180">
         <f>C33+C34</f>
-        <v>25799.699999999997</v>
+        <v>26232.739999999998</v>
       </c>
       <c r="I2" s="180"/>
       <c r="J2" s="180"/>
@@ -20021,7 +20327,9 @@
       <c r="B3" s="47">
         <v>52354.46</v>
       </c>
-      <c r="C3" s="191"/>
+      <c r="C3" s="191">
+        <v>300</v>
+      </c>
       <c r="D3" s="191">
         <v>2891.88</v>
       </c>
@@ -20029,7 +20337,7 @@
         <v>2891.88</v>
       </c>
       <c r="F3" s="191" t="s">
-        <v>278</v>
+        <v>692</v>
       </c>
       <c r="I3" s="47"/>
       <c r="J3" s="47"/>
@@ -20130,7 +20438,7 @@
     </row>
     <row r="5" spans="1:31" ht="16.5" thickTop="1" thickBot="1">
       <c r="C5" s="191">
-        <v>754.37</v>
+        <v>887.41</v>
       </c>
       <c r="D5" s="191">
         <v>754.37</v>
@@ -20203,6 +20511,10 @@
       <c r="F7" s="191" t="s">
         <v>138</v>
       </c>
+      <c r="H7">
+        <f>A2-48929.4</f>
+        <v>3271.8199999999997</v>
+      </c>
       <c r="K7" s="213"/>
       <c r="L7" s="213"/>
       <c r="M7" s="213"/>
@@ -20290,7 +20602,7 @@
         <v>598</v>
       </c>
       <c r="F10" s="191" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="K10" s="213"/>
       <c r="L10" s="213"/>
@@ -20410,7 +20722,7 @@
       </c>
       <c r="E14" s="134"/>
       <c r="F14" s="134" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G14" s="47"/>
       <c r="K14" s="213"/>
@@ -20876,7 +21188,7 @@
         <v>461</v>
       </c>
       <c r="C30" s="206">
-        <v>2800</v>
+        <v>2500</v>
       </c>
       <c r="D30" s="206">
         <v>1500</v>
@@ -20885,7 +21197,7 @@
         <v>1500</v>
       </c>
       <c r="F30" t="s">
-        <v>673</v>
+        <v>693</v>
       </c>
       <c r="K30" s="24"/>
       <c r="L30" s="208"/>
@@ -20953,7 +21265,9 @@
         <f>SUM(E19:E25)</f>
         <v>13076</v>
       </c>
-      <c r="F32" s="47"/>
+      <c r="F32" t="s">
+        <v>694</v>
+      </c>
       <c r="H32" s="180" t="s">
         <v>582</v>
       </c>
@@ -20982,7 +21296,7 @@
       </c>
       <c r="C33" s="200">
         <f>SUM(C2:C13)</f>
-        <v>5467.03</v>
+        <v>5900.0700000000006</v>
       </c>
       <c r="D33" s="200">
         <f>SUM(D2:D13)</f>
@@ -20997,7 +21311,7 @@
       </c>
       <c r="H33" s="180">
         <f>C33+C34</f>
-        <v>25799.699999999997</v>
+        <v>26232.739999999998</v>
       </c>
       <c r="I33" s="180"/>
       <c r="J33" s="180"/>
@@ -21090,7 +21404,7 @@
       </c>
       <c r="C36" s="245">
         <f>SUM(C30:C35)</f>
-        <v>48179.7</v>
+        <v>48312.74</v>
       </c>
       <c r="D36" s="245">
         <f>SUM(D30:D35)</f>
@@ -21126,7 +21440,7 @@
       </c>
       <c r="C37" s="154">
         <f>A2-C36</f>
-        <v>4021.5200000000041</v>
+        <v>3888.4800000000032</v>
       </c>
       <c r="D37" s="154">
         <f>A2-D36</f>
@@ -21401,9 +21715,11 @@
     </row>
     <row r="46" spans="1:32" ht="16.5" thickTop="1" thickBot="1">
       <c r="A46" t="s">
-        <v>674</v>
-      </c>
-      <c r="B46" s="47"/>
+        <v>672</v>
+      </c>
+      <c r="B46" s="47">
+        <v>27761040927</v>
+      </c>
       <c r="C46" s="47">
         <v>4</v>
       </c>
@@ -21529,7 +21845,10 @@
       </c>
       <c r="D49" s="47"/>
       <c r="E49" s="47"/>
-      <c r="F49" s="47"/>
+      <c r="F49" s="47">
+        <f>270*3</f>
+        <v>810</v>
+      </c>
       <c r="H49" t="s">
         <v>523</v>
       </c>
@@ -22486,7 +22805,7 @@
       </c>
       <c r="V86" s="235">
         <f>C2+E3+C4+C5+C26+C10+C11+C12+C17+C16+C22+C8+C6+C34</f>
-        <v>34192.58</v>
+        <v>34325.619999999995</v>
       </c>
       <c r="W86" s="235" t="e">
         <f>E2+#REF!+E4+E7+E26+E10+E11+E12+E13+E15+E17+E23+E8+E6+E27</f>
@@ -22550,7 +22869,7 @@
       </c>
       <c r="V87" s="115">
         <f>SUM(V5:V86)</f>
-        <v>34192.58</v>
+        <v>34325.619999999995</v>
       </c>
       <c r="W87" s="115">
         <f>SUM(W5:W85)</f>
@@ -22614,7 +22933,7 @@
       </c>
       <c r="V88" s="141">
         <f>V2-V87-V4+V3</f>
-        <v>114.7599999999984</v>
+        <v>-18.279999999995198</v>
       </c>
       <c r="W88" s="141">
         <f>W2+SUM(W5:W85)-W4</f>
@@ -22670,23 +22989,23 @@
       </c>
       <c r="V89" s="61">
         <f>SUM(O88:V88)</f>
-        <v>309393.75</v>
+        <v>309260.71000000002</v>
       </c>
       <c r="W89" s="61">
         <f>SUM(O88:W88)</f>
-        <v>358323.15</v>
+        <v>358190.11000000004</v>
       </c>
       <c r="X89" s="61">
         <f>SUM(O88:X88)</f>
-        <v>407252.55000000005</v>
+        <v>407119.51000000007</v>
       </c>
       <c r="Y89" s="61">
         <f>SUM(O88:Y88)</f>
-        <v>456181.95000000007</v>
+        <v>456048.91000000009</v>
       </c>
       <c r="Z89" s="61">
         <f>SUM(O88:Z88)</f>
-        <v>505186.35000000009</v>
+        <v>505053.31000000011</v>
       </c>
     </row>
     <row r="90" spans="8:31">
@@ -23250,8 +23569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6B59423-65C6-41E5-9225-5D345367A685}">
   <dimension ref="A1:AE111"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>